<commit_message>
[RF GEN]CPU SCH update
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V1.0/RF Generator Review Data_20190808.xlsx
+++ b/1_Schematic/Build V1.0/RF Generator Review Data_20190808.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,19 +11,90 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>VIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,19 +117,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,37 +420,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>48</v>
+      </c>
+      <c r="E5">
+        <f>48*0.8</f>
+        <v>38.400000000000006</v>
+      </c>
+      <c r="F5">
+        <f>48*1.2</f>
+        <v>57.599999999999994</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4.99</v>
+      </c>
+      <c r="E7">
+        <v>4.99</v>
+      </c>
+      <c r="F7">
+        <v>4.99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <f>D5/(D6+D7)</f>
+        <v>1.9207683073229289</v>
+      </c>
+      <c r="E8" s="1">
+        <f>E5/(E6+E7)</f>
+        <v>1.5366146458583434</v>
+      </c>
+      <c r="F8" s="1">
+        <f>F5/(F6+F7)</f>
+        <v>2.3049219687875144</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <f>D5*D8/1000</f>
+        <v>9.2196878751500594E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <f>E5*E8/1000</f>
+        <v>5.9006002400960399E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>F5*F8/1000</f>
+        <v>0.13276350540216084</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D5*D7/(D6+D7)</f>
+        <v>9.5846338535414155</v>
+      </c>
+      <c r="E10" s="1">
+        <f>E5*E7/(E6+E7)</f>
+        <v>7.6677070828331342</v>
+      </c>
+      <c r="F10" s="1">
+        <f>F5*F7/(F6+F7)</f>
+        <v>11.501560624249699</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>